<commit_message>
updated the manual review
</commit_message>
<xml_diff>
--- a/inst/app/www/lkselectedrecs_cleaned.xlsx
+++ b/inst/app/www/lkselectedrecs_cleaned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bach\Dropbox\Shiny\ShinyLink\inst\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E027BF-E452-4FFD-8E8D-7DAB4481BF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F843D765-68A5-4923-83D6-B00B54FEB68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4370" yWindow="4100" windowWidth="28800" windowHeight="15370" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1180,17 +1180,17 @@
   <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>